<commit_message>
Ex2 - 20. commit
</commit_message>
<xml_diff>
--- a/Ex2/measurement.xlsx
+++ b/Ex2/measurement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskjaer/Downloads/github/RobotEksperimentarium/Ex2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4537FFF-C329-0B43-A914-CDA9854F4FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2233B329-D63E-C842-A6C7-7688D5107AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16280" xr2:uid="{063E389B-44CA-0E43-8E99-A94BE855F4F8}"/>
   </bookViews>
@@ -109,6 +109,1093 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.617023192555476"/>
+                  <c:y val="-3.5539120362991061E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>y = x + 1</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>R² = 1</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2000"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ark1'!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ark1'!$C$2:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D649-7B46-A85F-87442E0BE4AB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="609403888"/>
+        <c:axId val="609405616"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="609403888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609405616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="609405616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="609403888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0115DE1-C01C-C314-8346-AFDFE64F04E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,148 +1495,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B47F735-0602-354C-98B6-27FFCD2521C7}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>300</v>
+      </c>
+      <c r="C22">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>300</v>
+      </c>
+      <c r="C23">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>300</v>
+      </c>
+      <c r="C24">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>300</v>
+      </c>
+      <c r="C25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
+      <c r="B26">
+        <v>300</v>
+      </c>
+      <c r="C26">
+        <v>301</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ex2 - 38. commit
</commit_message>
<xml_diff>
--- a/Ex2/measurement.xlsx
+++ b/Ex2/measurement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskjaer/Downloads/github/RobotEksperimentarium/Ex2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2233B329-D63E-C842-A6C7-7688D5107AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E6512E-8765-A543-B455-1EB13E54F9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16280" xr2:uid="{063E389B-44CA-0E43-8E99-A94BE855F4F8}"/>
   </bookViews>
@@ -53,10 +53,10 @@
     <t>300cm</t>
   </si>
   <si>
-    <t>Væg</t>
+    <t>Ben</t>
   </si>
   <si>
-    <t>Ben</t>
+    <t>Cardboardbox</t>
   </si>
 </sst>
 </file>
@@ -1498,17 +1498,20 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ex2 - 53. commit
</commit_message>
<xml_diff>
--- a/Ex2/measurement.xlsx
+++ b/Ex2/measurement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaskjaer/Downloads/github/RobotEksperimentarium/Ex2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E6512E-8765-A543-B455-1EB13E54F9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E983D-BFE3-0345-A9EF-9543F19DF19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16280" xr2:uid="{063E389B-44CA-0E43-8E99-A94BE855F4F8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
   <si>
     <t xml:space="preserve">10cm </t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>300cm</t>
-  </si>
-  <si>
-    <t>Ben</t>
   </si>
   <si>
     <t>Cardboardbox</t>
@@ -330,79 +327,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51</c:v>
+                  <c:v>50.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51</c:v>
+                  <c:v>50.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>50.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51</c:v>
+                  <c:v>50.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>101</c:v>
+                  <c:v>100.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>101</c:v>
+                  <c:v>100.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>101</c:v>
+                  <c:v>100.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>101</c:v>
+                  <c:v>100.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>101</c:v>
+                  <c:v>100.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>201</c:v>
+                  <c:v>201.2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>201</c:v>
+                  <c:v>201.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>201</c:v>
+                  <c:v>201.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>201</c:v>
+                  <c:v>201.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>201</c:v>
+                  <c:v>201.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>301</c:v>
+                  <c:v>298.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>301</c:v>
+                  <c:v>298.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>301</c:v>
+                  <c:v>298.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>301</c:v>
+                  <c:v>298.3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>301</c:v>
+                  <c:v>298.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B47F735-0602-354C-98B6-27FFCD2521C7}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1506,15 +1503,12 @@
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1522,10 +1516,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1533,10 +1527,10 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1544,10 +1538,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1555,10 +1549,10 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1566,10 +1560,10 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1580,7 +1574,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1588,10 +1582,10 @@
         <v>50</v>
       </c>
       <c r="C8">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1599,10 +1593,10 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1610,10 +1604,10 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1621,10 +1615,10 @@
         <v>50</v>
       </c>
       <c r="C11">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1632,10 +1626,10 @@
         <v>100</v>
       </c>
       <c r="C12">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1643,10 +1637,10 @@
         <v>100</v>
       </c>
       <c r="C13">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1654,10 +1648,10 @@
         <v>100</v>
       </c>
       <c r="C14">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1665,10 +1659,10 @@
         <v>100</v>
       </c>
       <c r="C15">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1676,7 +1670,7 @@
         <v>100</v>
       </c>
       <c r="C16">
-        <v>101</v>
+        <v>100.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1687,7 +1681,7 @@
         <v>200</v>
       </c>
       <c r="C17">
-        <v>201</v>
+        <v>201.2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1698,7 +1692,7 @@
         <v>200</v>
       </c>
       <c r="C18">
-        <v>201</v>
+        <v>201.2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1709,7 +1703,7 @@
         <v>200</v>
       </c>
       <c r="C19">
-        <v>201</v>
+        <v>201.2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1720,7 +1714,7 @@
         <v>200</v>
       </c>
       <c r="C20">
-        <v>201</v>
+        <v>201.2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1731,7 +1725,7 @@
         <v>200</v>
       </c>
       <c r="C21">
-        <v>201</v>
+        <v>201.2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1742,7 +1736,7 @@
         <v>300</v>
       </c>
       <c r="C22">
-        <v>301</v>
+        <v>298.39999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1753,7 +1747,7 @@
         <v>300</v>
       </c>
       <c r="C23">
-        <v>301</v>
+        <v>298.39999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1764,7 +1758,7 @@
         <v>300</v>
       </c>
       <c r="C24">
-        <v>301</v>
+        <v>298.3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1775,7 +1769,7 @@
         <v>300</v>
       </c>
       <c r="C25">
-        <v>301</v>
+        <v>298.3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1786,7 +1780,7 @@
         <v>300</v>
       </c>
       <c r="C26">
-        <v>301</v>
+        <v>298.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>